<commit_message>
Section 28: Protecting Excel Worksheets and Workbooks
</commit_message>
<xml_diff>
--- a/Section 28: Protecting Excel Worksheets and Workbooks/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 28: Protecting Excel Worksheets and Workbooks/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 28: Protecting Excel Worksheets and Workbooks/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A558DDCE-B4CA-744D-87A3-AB87974C9210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D553B2-85D7-9645-AD6D-FC229240A58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16880" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16780" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -1628,7 +1629,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1946,6 +1947,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="13" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1964,83 +1972,17 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2754,14 +2696,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1"/>
     <row r="2" spans="1:9" ht="17" thickBot="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="131" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2958,13 +2900,13 @@
       <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="125" t="s">
+      <c r="A12" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="126"/>
-      <c r="C12" s="126"/>
-      <c r="D12" s="126"/>
-      <c r="E12" s="127"/>
+      <c r="B12" s="129"/>
+      <c r="C12" s="129"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -3104,10 +3046,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="131" t="s">
+      <c r="E2" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="131"/>
+      <c r="F2" s="136"/>
     </row>
     <row r="3" spans="2:6" ht="14">
       <c r="B3" s="25" t="s">
@@ -3116,11 +3058,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="132" t="str">
+      <c r="E3" s="134" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="133"/>
+      <c r="F3" s="135"/>
     </row>
     <row r="4" spans="2:6" ht="14">
       <c r="B4" s="25" t="s">
@@ -3129,11 +3071,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="132" t="str">
+      <c r="E4" s="134" t="str">
         <f>_xlfn.CONCAT(C4, " ", B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="133"/>
+      <c r="F4" s="135"/>
     </row>
     <row r="5" spans="2:6" ht="14">
       <c r="B5" s="25" t="s">
@@ -3142,11 +3084,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="132" t="str">
+      <c r="E5" s="134" t="str">
         <f t="shared" ref="E5:E17" si="0">_xlfn.CONCAT(C5, " ", B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="133"/>
+      <c r="F5" s="135"/>
     </row>
     <row r="6" spans="2:6" ht="14">
       <c r="B6" s="25" t="s">
@@ -3155,11 +3097,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="132" t="str">
+      <c r="E6" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="133"/>
+      <c r="F6" s="135"/>
     </row>
     <row r="7" spans="2:6" ht="14">
       <c r="B7" s="25" t="s">
@@ -3168,11 +3110,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="132" t="str">
+      <c r="E7" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="133"/>
+      <c r="F7" s="135"/>
     </row>
     <row r="8" spans="2:6" ht="14">
       <c r="B8" s="25" t="s">
@@ -3181,11 +3123,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="132" t="str">
+      <c r="E8" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="133"/>
+      <c r="F8" s="135"/>
     </row>
     <row r="9" spans="2:6" ht="14">
       <c r="B9" s="25" t="s">
@@ -3194,11 +3136,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="132" t="str">
+      <c r="E9" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="133"/>
+      <c r="F9" s="135"/>
     </row>
     <row r="10" spans="2:6" ht="14">
       <c r="B10" s="25" t="s">
@@ -3207,11 +3149,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="132" t="str">
+      <c r="E10" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="133"/>
+      <c r="F10" s="135"/>
     </row>
     <row r="11" spans="2:6" ht="14">
       <c r="B11" s="25" t="s">
@@ -3220,11 +3162,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="132" t="str">
+      <c r="E11" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="133"/>
+      <c r="F11" s="135"/>
     </row>
     <row r="12" spans="2:6" ht="14">
       <c r="B12" s="25" t="s">
@@ -3233,11 +3175,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="132" t="str">
+      <c r="E12" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="133"/>
+      <c r="F12" s="135"/>
     </row>
     <row r="13" spans="2:6" ht="14">
       <c r="B13" s="25" t="s">
@@ -3246,11 +3188,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="132" t="str">
+      <c r="E13" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="133"/>
+      <c r="F13" s="135"/>
     </row>
     <row r="14" spans="2:6" ht="14">
       <c r="B14" s="25" t="s">
@@ -3259,11 +3201,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="132" t="str">
+      <c r="E14" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="133"/>
+      <c r="F14" s="135"/>
     </row>
     <row r="15" spans="2:6" ht="14">
       <c r="B15" s="25" t="s">
@@ -3272,11 +3214,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="132" t="str">
+      <c r="E15" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="133"/>
+      <c r="F15" s="135"/>
     </row>
     <row r="16" spans="2:6" ht="14">
       <c r="B16" s="25" t="s">
@@ -3285,11 +3227,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="132" t="str">
+      <c r="E16" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="133"/>
+      <c r="F16" s="135"/>
     </row>
     <row r="17" spans="2:6" ht="14">
       <c r="B17" s="25" t="s">
@@ -3298,11 +3240,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="132" t="str">
+      <c r="E17" s="134" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="133"/>
+      <c r="F17" s="135"/>
     </row>
     <row r="18" spans="2:6" ht="14">
       <c r="B18" s="25" t="s">
@@ -3311,21 +3253,14 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="132" t="str">
+      <c r="E18" s="134" t="str">
         <f>_xlfn.CONCAT(C18, " ", B18)</f>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="133"/>
+      <c r="F18" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3336,6 +3271,13 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3348,70 +3290,69 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="135" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="135" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="135" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="135" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="135" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="135" customWidth="1"/>
-    <col min="7" max="7" width="1.1640625" style="135" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" style="135" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" style="135" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="135"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="1.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1"/>
     <row r="2" spans="1:9" ht="17" thickBot="1">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="131" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="136"/>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="H2" s="137" t="s">
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="138">
+      <c r="I2" s="125">
         <v>34000</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" thickTop="1" thickBot="1"/>
     <row r="4" spans="1:9" ht="14">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="140" t="s">
+      <c r="C4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="140" t="s">
+      <c r="D4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="140" t="s">
+      <c r="E4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="141" t="s">
+      <c r="F4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="142" t="s">
+      <c r="H4" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="143" t="s">
+      <c r="I4" s="52" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="72">
@@ -3426,21 +3367,21 @@
       <c r="E5" s="72">
         <v>8965</v>
       </c>
-      <c r="F5" s="145">
+      <c r="F5" s="126">
         <f>SUM(B5:E5)</f>
         <v>36245</v>
       </c>
-      <c r="H5" s="146" t="str">
+      <c r="H5" s="1" t="str">
         <f>IF(F5&gt;=$I$2,"YES", "NO")</f>
         <v>YES</v>
       </c>
-      <c r="I5" s="147" t="str">
+      <c r="I5" s="2" t="str">
         <f>IF(AND(H5="YES", MIN(B5:E5)&gt;=8000), "BONUS", "NO BONUS")</f>
         <v>BONUS</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="72">
@@ -3455,21 +3396,21 @@
       <c r="E6" s="72">
         <v>10100</v>
       </c>
-      <c r="F6" s="145">
+      <c r="F6" s="126">
         <f>SUM(B6:E6)</f>
         <v>31475</v>
       </c>
-      <c r="H6" s="146" t="str">
+      <c r="H6" s="1" t="str">
         <f t="shared" ref="H6:H9" si="0">IF(F6&gt;=$I$2,"YES", "NO")</f>
         <v>NO</v>
       </c>
-      <c r="I6" s="147" t="str">
+      <c r="I6" s="2" t="str">
         <f t="shared" ref="I6:I9" si="1">IF(AND(H6="YES", MIN(B6:E6)&gt;=8000), "BONUS", "NO BONUS")</f>
         <v>NO BONUS</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="72">
@@ -3484,21 +3425,21 @@
       <c r="E7" s="72">
         <v>7512</v>
       </c>
-      <c r="F7" s="145">
+      <c r="F7" s="126">
         <f>SUM(B7:E7)</f>
         <v>33427</v>
       </c>
-      <c r="H7" s="146" t="str">
+      <c r="H7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NO</v>
       </c>
-      <c r="I7" s="147" t="str">
+      <c r="I7" s="2" t="str">
         <f t="shared" si="1"/>
         <v>NO BONUS</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16">
-      <c r="A8" s="144" t="s">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="72">
@@ -3513,21 +3454,21 @@
       <c r="E8" s="72">
         <v>9795</v>
       </c>
-      <c r="F8" s="145">
+      <c r="F8" s="126">
         <f>SUM(B8:E8)</f>
         <v>39705</v>
       </c>
-      <c r="H8" s="146" t="str">
+      <c r="H8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>YES</v>
       </c>
-      <c r="I8" s="147" t="str">
+      <c r="I8" s="2" t="str">
         <f t="shared" si="1"/>
         <v>BONUS</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" thickBot="1">
-      <c r="A9" s="148" t="s">
+      <c r="A9" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="73">
@@ -3542,66 +3483,66 @@
       <c r="E9" s="73">
         <v>10252</v>
       </c>
-      <c r="F9" s="149">
+      <c r="F9" s="127">
         <f>SUM(B9:E9)</f>
         <v>35359</v>
       </c>
-      <c r="H9" s="146" t="str">
+      <c r="H9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>YES</v>
       </c>
-      <c r="I9" s="147" t="str">
+      <c r="I9" s="2" t="str">
         <f t="shared" si="1"/>
         <v>NO BONUS</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="48" t="s">
         <v>223</v>
       </c>
-      <c r="B10" s="151">
+      <c r="B10" s="53">
         <f>SUM(B5:B9)</f>
         <v>40402</v>
       </c>
-      <c r="C10" s="151">
+      <c r="C10" s="53">
         <f t="shared" ref="C10:F10" si="2">SUM(C5:C9)</f>
         <v>42555</v>
       </c>
-      <c r="D10" s="151">
+      <c r="D10" s="53">
         <f t="shared" si="2"/>
         <v>46630</v>
       </c>
-      <c r="E10" s="151">
+      <c r="E10" s="53">
         <f t="shared" si="2"/>
         <v>46624</v>
       </c>
-      <c r="F10" s="151">
+      <c r="F10" s="53">
         <f t="shared" si="2"/>
         <v>176211</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14">
-      <c r="A11" s="152"/>
+      <c r="A11" s="49"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
-      <c r="E12" s="153" t="s">
+      <c r="E12" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="154">
+      <c r="F12" s="4">
         <f>SUM(F5:F10)</f>
         <v>352422</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="155" t="s">
+      <c r="A14" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="156"/>
-      <c r="C14" s="156"/>
-      <c r="D14" s="156"/>
-      <c r="E14" s="157"/>
-      <c r="F14" s="158">
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
       </c>
@@ -3671,14 +3612,14 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14" thickBot="1"/>
     <row r="2" spans="1:9" ht="17" thickBot="1">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="131" t="s">
         <v>222</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
       <c r="H2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3898,13 +3839,13 @@
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1"/>
     <row r="14" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A14" s="125" t="s">
+      <c r="A14" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="126"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="127"/>
+      <c r="B14" s="129"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="3">
         <f>COUNTIF(H5:H9, "YES")</f>
         <v>3</v>
@@ -4450,10 +4391,10 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="134" t="s">
+      <c r="B10" s="137" t="s">
         <v>259</v>
       </c>
-      <c r="C10" s="134"/>
+      <c r="C10" s="137"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="114" t="s">
@@ -13175,10 +13116,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14" thickBot="1"/>
     <row r="2" spans="1:2" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="132" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="130"/>
+      <c r="B2" s="133"/>
     </row>
     <row r="3" spans="1:2" ht="18" thickTop="1" thickBot="1">
       <c r="A3" s="61" t="s">
@@ -13345,8 +13286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
Working with Excel's Solver Tool
</commit_message>
<xml_diff>
--- a/Section 28: Protecting Excel Worksheets and Workbooks/Resources/Excel103-AdvancedExercises.xlsx
+++ b/Section 28: Protecting Excel Worksheets and Workbooks/Resources/Excel103-AdvancedExercises.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolinecrandell/Documents/Employment/*Applications/2022.12 Job Apps/GitHub/excel/Section 28: Protecting Excel Worksheets and Workbooks/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D553B2-85D7-9645-AD6D-FC229240A58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23100AD3-0BA8-8342-90C1-24094BD0B9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16780" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="16780" firstSheet="9" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IF Function" sheetId="4" r:id="rId1"/>
@@ -40,21 +40,22 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Master Emp List'!$B$1:$I$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SUMIF Function'!$A$2:$E$272</definedName>
     <definedName name="Monthly_Goal">'IF Function'!$I$2</definedName>
+    <definedName name="solver_adj" localSheetId="15" hidden="1">Solver!$B$5:$E$7</definedName>
     <definedName name="solver_cvg" localSheetId="15" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="15" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs2" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs3" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="15" hidden="1">Solver!$B$5:$E$5</definedName>
+    <definedName name="solver_lhs2" localSheetId="15" hidden="1">Solver!$B$5:$E$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="15" hidden="1">Solver!$B$6:$E$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="15" hidden="1">Solver!$B$7:$E$7</definedName>
     <definedName name="solver_lhs5" localSheetId="15" hidden="1">Solver!$B$8:$E$8</definedName>
     <definedName name="solver_lhs6" localSheetId="15" hidden="1">Solver!$E$8</definedName>
     <definedName name="solver_lhs7" localSheetId="15" hidden="1">Solver!$E$8</definedName>
     <definedName name="solver_lhs8" localSheetId="15" hidden="1">Solver!$E$8</definedName>
-    <definedName name="solver_lin" localSheetId="15" hidden="1">0</definedName>
+    <definedName name="solver_lin" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="15" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="15" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="15" hidden="1">0.075</definedName>
@@ -63,24 +64,24 @@
     <definedName name="solver_neg" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="15" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="15" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="15" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'IF Function'!$I$2</definedName>
     <definedName name="solver_opt" localSheetId="15" hidden="1">Solver!$H$8</definedName>
     <definedName name="solver_pre" localSheetId="15" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="15" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel3" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rel4" localSheetId="15" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="15" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="15" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="15" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="15" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_rel6" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_rel7" localSheetId="15" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="15" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs2" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs3" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="15" hidden="1">92</definedName>
+    <definedName name="solver_rhs2" localSheetId="15" hidden="1">20</definedName>
+    <definedName name="solver_rhs3" localSheetId="15" hidden="1">45</definedName>
+    <definedName name="solver_rhs4" localSheetId="15" hidden="1">55</definedName>
     <definedName name="solver_rhs5" localSheetId="15" hidden="1">Solver!$B$10:$E$10</definedName>
     <definedName name="solver_rhs6" localSheetId="15" hidden="1">Solver!$E$10</definedName>
     <definedName name="solver_rhs7" localSheetId="15" hidden="1">Solver!$E$10</definedName>
@@ -97,7 +98,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="15" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="15" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="15" hidden="1">2</definedName>
     <definedName name="Week_1">'IF Function'!$B$5:$B$9</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1972,13 +1973,13 @@
     <xf numFmtId="0" fontId="16" fillId="8" borderId="17" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3046,10 +3047,10 @@
       <c r="C2" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="136" t="s">
+      <c r="E2" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="136"/>
+      <c r="F2" s="134"/>
     </row>
     <row r="3" spans="2:6" ht="14">
       <c r="B3" s="25" t="s">
@@ -3058,11 +3059,11 @@
       <c r="C3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="134" t="str">
+      <c r="E3" s="135" t="str">
         <f>CONCATENATE(C3," ",B3)</f>
         <v>Howard Smith</v>
       </c>
-      <c r="F3" s="135"/>
+      <c r="F3" s="136"/>
     </row>
     <row r="4" spans="2:6" ht="14">
       <c r="B4" s="25" t="s">
@@ -3071,11 +3072,11 @@
       <c r="C4" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="134" t="str">
+      <c r="E4" s="135" t="str">
         <f>_xlfn.CONCAT(C4, " ", B4)</f>
         <v>Joe Gonzales</v>
       </c>
-      <c r="F4" s="135"/>
+      <c r="F4" s="136"/>
     </row>
     <row r="5" spans="2:6" ht="14">
       <c r="B5" s="25" t="s">
@@ -3084,11 +3085,11 @@
       <c r="C5" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="134" t="str">
+      <c r="E5" s="135" t="str">
         <f t="shared" ref="E5:E17" si="0">_xlfn.CONCAT(C5, " ", B5)</f>
         <v>Gail Scote</v>
       </c>
-      <c r="F5" s="135"/>
+      <c r="F5" s="136"/>
     </row>
     <row r="6" spans="2:6" ht="14">
       <c r="B6" s="25" t="s">
@@ -3097,11 +3098,11 @@
       <c r="C6" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="134" t="str">
+      <c r="E6" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sheryl Kane</v>
       </c>
-      <c r="F6" s="135"/>
+      <c r="F6" s="136"/>
     </row>
     <row r="7" spans="2:6" ht="14">
       <c r="B7" s="25" t="s">
@@ -3110,11 +3111,11 @@
       <c r="C7" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="134" t="str">
+      <c r="E7" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Kendrick Hapsbuch</v>
       </c>
-      <c r="F7" s="135"/>
+      <c r="F7" s="136"/>
     </row>
     <row r="8" spans="2:6" ht="14">
       <c r="B8" s="25" t="s">
@@ -3123,11 +3124,11 @@
       <c r="C8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="134" t="str">
+      <c r="E8" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Mark Henders</v>
       </c>
-      <c r="F8" s="135"/>
+      <c r="F8" s="136"/>
     </row>
     <row r="9" spans="2:6" ht="14">
       <c r="B9" s="25" t="s">
@@ -3136,11 +3137,11 @@
       <c r="C9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="134" t="str">
+      <c r="E9" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Katie Atherton</v>
       </c>
-      <c r="F9" s="135"/>
+      <c r="F9" s="136"/>
     </row>
     <row r="10" spans="2:6" ht="14">
       <c r="B10" s="25" t="s">
@@ -3149,11 +3150,11 @@
       <c r="C10" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="134" t="str">
+      <c r="E10" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Frank Bellwood</v>
       </c>
-      <c r="F10" s="135"/>
+      <c r="F10" s="136"/>
     </row>
     <row r="11" spans="2:6" ht="14">
       <c r="B11" s="25" t="s">
@@ -3162,11 +3163,11 @@
       <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="134" t="str">
+      <c r="E11" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Linda Cooper</v>
       </c>
-      <c r="F11" s="135"/>
+      <c r="F11" s="136"/>
     </row>
     <row r="12" spans="2:6" ht="14">
       <c r="B12" s="25" t="s">
@@ -3175,11 +3176,11 @@
       <c r="C12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="134" t="str">
+      <c r="E12" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Brent Cronwith</v>
       </c>
-      <c r="F12" s="135"/>
+      <c r="F12" s="136"/>
     </row>
     <row r="13" spans="2:6" ht="14">
       <c r="B13" s="25" t="s">
@@ -3188,11 +3189,11 @@
       <c r="C13" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="134" t="str">
+      <c r="E13" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Sandrae Simpson</v>
       </c>
-      <c r="F13" s="135"/>
+      <c r="F13" s="136"/>
     </row>
     <row r="14" spans="2:6" ht="14">
       <c r="B14" s="25" t="s">
@@ -3201,11 +3202,11 @@
       <c r="C14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="134" t="str">
+      <c r="E14" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Randy Sindole</v>
       </c>
-      <c r="F14" s="135"/>
+      <c r="F14" s="136"/>
     </row>
     <row r="15" spans="2:6" ht="14">
       <c r="B15" s="25" t="s">
@@ -3214,11 +3215,11 @@
       <c r="C15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="134" t="str">
+      <c r="E15" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Ellen Smith</v>
       </c>
-      <c r="F15" s="135"/>
+      <c r="F15" s="136"/>
     </row>
     <row r="16" spans="2:6" ht="14">
       <c r="B16" s="25" t="s">
@@ -3227,11 +3228,11 @@
       <c r="C16" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="134" t="str">
+      <c r="E16" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tuome Vuanuo</v>
       </c>
-      <c r="F16" s="135"/>
+      <c r="F16" s="136"/>
     </row>
     <row r="17" spans="2:6" ht="14">
       <c r="B17" s="25" t="s">
@@ -3240,11 +3241,11 @@
       <c r="C17" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="134" t="str">
+      <c r="E17" s="135" t="str">
         <f t="shared" si="0"/>
         <v>Tadeuz Szcznyck</v>
       </c>
-      <c r="F17" s="135"/>
+      <c r="F17" s="136"/>
     </row>
     <row r="18" spans="2:6" ht="14">
       <c r="B18" s="25" t="s">
@@ -3253,14 +3254,21 @@
       <c r="C18" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="134" t="str">
+      <c r="E18" s="135" t="str">
         <f>_xlfn.CONCAT(C18, " ", B18)</f>
         <v>Tammy Wu</v>
       </c>
-      <c r="F18" s="135"/>
+      <c r="F18" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
@@ -3271,13 +3279,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3921,8 +3922,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -3985,16 +3986,16 @@
         <v>271</v>
       </c>
       <c r="B5" s="86">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C5" s="86">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D5" s="86">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E5" s="86">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F5" s="74"/>
       <c r="G5" s="85">
@@ -4002,7 +4003,7 @@
       </c>
       <c r="H5" s="84">
         <f>G5*(B5+C5+D5+E5)</f>
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16">
@@ -4010,16 +4011,16 @@
         <v>270</v>
       </c>
       <c r="B6" s="88">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C6" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E6" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F6" s="74"/>
       <c r="G6" s="85">
@@ -4027,7 +4028,7 @@
       </c>
       <c r="H6" s="84">
         <f>G6*(B6+C6+D6+E6)</f>
-        <v>0</v>
+        <v>147.20000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16">
@@ -4035,16 +4036,16 @@
         <v>269</v>
       </c>
       <c r="B7" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C7" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D7" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E7" s="86">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F7" s="74"/>
       <c r="G7" s="85">
@@ -4052,7 +4053,7 @@
       </c>
       <c r="H7" s="84">
         <f>G7*(B7+C7+D7+E7)</f>
-        <v>0</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16">
@@ -4061,25 +4062,25 @@
       </c>
       <c r="B8" s="83">
         <f>SUM(B5:B7)</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C8" s="83">
         <f>SUM(C5:C7)</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D8" s="83">
         <f>SUM(D5:D7)</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="E8" s="83">
         <f>SUM(E5:E7)</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="F8" s="74"/>
       <c r="G8" s="82"/>
       <c r="H8" s="105">
         <f>H5+H6+H7</f>
-        <v>5</v>
+        <v>363.20000000000005</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="4.5" customHeight="1">
@@ -13286,7 +13287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A99380-3415-42C6-8C41-613698A280FA}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>

</xml_diff>